<commit_message>
Update to seed the DB
</commit_message>
<xml_diff>
--- a/ExemploExcel.xlsx
+++ b/ExemploExcel.xlsx
@@ -1,51 +1,225 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\LerExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\excel-para-sqlserve-aspnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E38DCDB-0C95-45A6-A8A9-47CBD5F09F5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4566BE-8B50-491B-96EC-24A37EFB17C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{86F04CBE-24D8-4DEA-BCA0-1E40CA1DFA96}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Descricao</t>
-  </si>
-  <si>
-    <t>Preco</t>
-  </si>
-  <si>
-    <t>Desktop</t>
-  </si>
-  <si>
-    <t>Notebook</t>
-  </si>
-  <si>
-    <t>HD Externo</t>
-  </si>
-  <si>
-    <t>Monitor</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+  <si>
+    <t>Aldenir Queiroz</t>
+  </si>
+  <si>
+    <t>Ambrosio</t>
+  </si>
+  <si>
+    <t>Anizio</t>
+  </si>
+  <si>
+    <t>Belarmino</t>
+  </si>
+  <si>
+    <t>Bene</t>
+  </si>
+  <si>
+    <t>Degmar</t>
+  </si>
+  <si>
+    <t>Dinho</t>
+  </si>
+  <si>
+    <t>Donizete Salamão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doutor  </t>
+  </si>
+  <si>
+    <t>Doutor colega</t>
+  </si>
+  <si>
+    <t>Edmar Oro Mon</t>
+  </si>
+  <si>
+    <t>Edvana</t>
+  </si>
+  <si>
+    <t>Eucilene</t>
+  </si>
+  <si>
+    <t>Gomes</t>
+  </si>
+  <si>
+    <t>Helim</t>
+  </si>
+  <si>
+    <t>Hermenegildo</t>
+  </si>
+  <si>
+    <t>Jaderson</t>
+  </si>
+  <si>
+    <t>Joaquina</t>
+  </si>
+  <si>
+    <t>Jose Basílio</t>
+  </si>
+  <si>
+    <t>José Poço</t>
+  </si>
+  <si>
+    <t>Jovanny</t>
+  </si>
+  <si>
+    <t>Leonildo</t>
+  </si>
+  <si>
+    <t>Luizão</t>
+  </si>
+  <si>
+    <t>Maria Helena</t>
+  </si>
+  <si>
+    <t>Neco</t>
+  </si>
+  <si>
+    <t>Olga Keila</t>
+  </si>
+  <si>
+    <t>Paulo Gonçalves</t>
+  </si>
+  <si>
+    <t>Pedaço</t>
+  </si>
+  <si>
+    <t>Raimunda Carmelo</t>
+  </si>
+  <si>
+    <t>Raul</t>
+  </si>
+  <si>
+    <t>Seabra</t>
+  </si>
+  <si>
+    <t>Souza</t>
+  </si>
+  <si>
+    <t>Tainara</t>
+  </si>
+  <si>
+    <t>Valdecir</t>
+  </si>
+  <si>
+    <t>Wilma</t>
+  </si>
+  <si>
+    <t>Ze</t>
+  </si>
+  <si>
+    <t>Nego Nega</t>
+  </si>
+  <si>
+    <t>Maiara Paz</t>
+  </si>
+  <si>
+    <t>Alissandreia</t>
+  </si>
+  <si>
+    <t>Aldenir</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Francisca</t>
+  </si>
+  <si>
+    <t>Edmar</t>
+  </si>
+  <si>
+    <t>mãe</t>
+  </si>
+  <si>
+    <t>Mãe</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Pai</t>
+  </si>
+  <si>
+    <t>Edvania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivone </t>
+  </si>
+  <si>
+    <t>Doutor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Esposa</t>
+  </si>
+  <si>
+    <t>Marilda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Neguinha</t>
+  </si>
+  <si>
+    <t>Milene</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gilberto</t>
+  </si>
+  <si>
+    <t>Esposa Irmã</t>
+  </si>
+  <si>
+    <t>Irmã</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lilito </t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nato</t>
+  </si>
+  <si>
+    <t>Keila</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Degmar</t>
   </si>
 </sst>
 </file>
@@ -81,11 +255,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -104,7 +275,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -120,7 +291,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -132,7 +303,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -149,7 +320,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -179,12 +350,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -214,6 +402,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -365,71 +570,348 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A7A7B5-5654-4968-9E90-3799E7E8760E}">
+  <dimension ref="A2:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
-        <v>600</v>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>